<commit_message>
Container is up and the database is connected.
</commit_message>
<xml_diff>
--- a/registro_de_usuarios.xlsx
+++ b/registro_de_usuarios.xlsx
@@ -212,7 +212,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,7 +242,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,7 +254,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>